<commit_message>
final changes to SAP task, only thing missing are new outcome slides
</commit_message>
<xml_diff>
--- a/task/+eventCreator/stimulus_randomisation.xlsx
+++ b/task/+eventCreator/stimulus_randomisation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwellste/projects/SEPAB/tasks/social_affective_prediction_task/task/+eventCreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109F983E-517C-DC42-8358-ED95D0BDAC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB937CD3-CA7D-8040-83CE-6AE0CF193D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30300" yWindow="540" windowWidth="34560" windowHeight="19940" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
+    <workbookView xWindow="45620" yWindow="500" windowWidth="34560" windowHeight="19940" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="16">
   <si>
     <t>f1</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>fmri_experiment_a3</t>
-  </si>
-  <si>
-    <t>fmri_experiment_a4</t>
   </si>
   <si>
     <t>m1</t>
@@ -129,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -166,31 +163,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -198,23 +175,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -246,18 +211,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0BC8E85C-457C-8A48-9CA8-1DF766781831}" name="Table1" displayName="Table1" ref="A1:I42" totalsRowShown="0">
-  <autoFilter ref="A1:I42" xr:uid="{0BC8E85C-457C-8A48-9CA8-1DF766781831}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{03EB077A-5165-9142-8C50-C55FE7B306DE}" name="PID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{EDE56B64-66C6-3040-AD71-0E6728092496}" name="behav_practice_a1"/>
-    <tableColumn id="3" xr3:uid="{24CF8084-0D39-D54D-8B3F-54E4D28BCF23}" name="behav_practice_a2"/>
-    <tableColumn id="4" xr3:uid="{CD72D285-AE14-DC47-8881-9AB285AFEE3F}" name="fmri_practice_a1"/>
-    <tableColumn id="5" xr3:uid="{EC42F437-0A7C-CD4B-AFD1-CCCDEE6C9C2B}" name="fmri_practice_a2"/>
-    <tableColumn id="6" xr3:uid="{5BBA8660-61F7-EE4F-BA66-70E62B7835FF}" name="fmri_experiment_a1" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{C4484F94-421C-E140-AC5B-637E12F31E3D}" name="fmri_experiment_a2"/>
-    <tableColumn id="8" xr3:uid="{8C857854-38AF-3243-9C36-E4BA65D83779}" name="fmri_experiment_a3"/>
-    <tableColumn id="9" xr3:uid="{218C89E1-4E87-0745-B216-F120DFC6AE6E}" name="fmri_experiment_a4" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2967624C-A5FB-5A44-9608-53655EE5D9E1}" name="Table13" displayName="Table13" ref="A1:H42" totalsRowShown="0">
+  <autoFilter ref="A1:H42" xr:uid="{2967624C-A5FB-5A44-9608-53655EE5D9E1}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9076E2B0-A52A-4F4C-A40D-59F7CFBAE5E1}" name="PID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{78B7B15E-BB00-8F4A-A432-63588FEDAAE2}" name="behav_practice_a1"/>
+    <tableColumn id="3" xr3:uid="{22060187-0CE8-E94A-9F48-5588CA3B8702}" name="behav_practice_a2"/>
+    <tableColumn id="4" xr3:uid="{ECE6ECD9-0A99-1140-86F9-81BDCCC84A63}" name="fmri_practice_a1"/>
+    <tableColumn id="5" xr3:uid="{A4867C1A-4C72-6046-85DF-FC0C5CA7A438}" name="fmri_practice_a2"/>
+    <tableColumn id="6" xr3:uid="{614B054E-B73B-3549-B094-878AB5B37ED8}" name="fmri_experiment_a1" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{C287A44E-7E0E-8949-90B7-BB37CB7BDF46}" name="fmri_experiment_a2"/>
+    <tableColumn id="8" xr3:uid="{66E5212A-86A8-D040-BD38-95AD739411D3}" name="fmri_experiment_a3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,20 +524,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886A73D-7D5B-1440-9AEF-D5255F093359}">
-  <dimension ref="A1:CK61"/>
+  <dimension ref="A1:CB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="9" width="20.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -596,11 +557,8 @@
       <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:80" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -608,26 +566,24 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -699,162 +655,138 @@
       <c r="BZ2"/>
       <c r="CA2"/>
       <c r="CB2"/>
-      <c r="CC2"/>
-      <c r="CD2"/>
-      <c r="CE2"/>
-      <c r="CF2"/>
-      <c r="CG2"/>
-      <c r="CH2"/>
-      <c r="CI2"/>
-      <c r="CJ2"/>
-      <c r="CK2"/>
-    </row>
-    <row r="3" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:89" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:89" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1004</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1005</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:89" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -862,57 +794,51 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1008</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:80" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -920,26 +846,24 @@
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -1011,46 +935,34 @@
       <c r="BZ10"/>
       <c r="CA10"/>
       <c r="CB10"/>
-      <c r="CC10"/>
-      <c r="CD10"/>
-      <c r="CE10"/>
-      <c r="CF10"/>
-      <c r="CG10"/>
-      <c r="CH10"/>
-      <c r="CI10"/>
-      <c r="CJ10"/>
-      <c r="CK10"/>
-    </row>
-    <row r="11" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1010</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:89" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1058,173 +970,155 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:89" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1012</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:89" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1013</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:89" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1014</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:89" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1015</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
         <v>0</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1016</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:80" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -1232,26 +1126,24 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
@@ -1323,46 +1215,34 @@
       <c r="BZ18"/>
       <c r="CA18"/>
       <c r="CB18"/>
-      <c r="CC18"/>
-      <c r="CD18"/>
-      <c r="CE18"/>
-      <c r="CF18"/>
-      <c r="CG18"/>
-      <c r="CH18"/>
-      <c r="CI18"/>
-      <c r="CJ18"/>
-      <c r="CK18"/>
-    </row>
-    <row r="19" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1018</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:89" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -1370,173 +1250,155 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:89" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1020</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:89" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1021</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:89" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1022</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
         <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:89" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1023</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
         <v>1</v>
       </c>
-      <c r="I24" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1024</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:89" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:80" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1025</v>
       </c>
@@ -1544,26 +1406,24 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>11</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26"/>
@@ -1635,22 +1495,13 @@
       <c r="BZ26"/>
       <c r="CA26"/>
       <c r="CB26"/>
-      <c r="CC26"/>
-      <c r="CD26"/>
-      <c r="CE26"/>
-      <c r="CF26"/>
-      <c r="CG26"/>
-      <c r="CH26"/>
-      <c r="CI26"/>
-      <c r="CJ26"/>
-      <c r="CK26"/>
-    </row>
-    <row r="27" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1026</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1659,33 +1510,30 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:89" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1027</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1694,103 +1542,91 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:89" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1028</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:89" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1029</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H30" t="s">
         <v>0</v>
       </c>
-      <c r="I30" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:89" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1030</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31" t="s">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:89" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:80" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1031</v>
       </c>
@@ -1798,57 +1634,51 @@
         <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H32" t="s">
         <v>1</v>
       </c>
-      <c r="I32" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1032</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1033</v>
       </c>
@@ -1856,91 +1686,82 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1034</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1035</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>12</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1036</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
@@ -1949,80 +1770,71 @@
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1037</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H38" t="s">
         <v>1</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1038</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1039</v>
       </c>
@@ -2030,87 +1842,75 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H40" t="s">
         <v>0</v>
       </c>
-      <c r="I40" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1040</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41" t="s">
         <v>1</v>
       </c>
       <c r="H41" t="s">
-        <v>10</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1041</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E61" s="2"/>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2136,16 +1936,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -2156,16 +1956,16 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -2176,16 +1976,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -2196,16 +1996,16 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -2216,16 +2016,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8">
         <v>8</v>
@@ -2236,16 +2036,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <v>8</v>
@@ -2256,16 +2056,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -2276,16 +2076,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11">
         <v>8</v>
@@ -2293,7 +2093,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -2302,10 +2102,10 @@
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13">
         <v>8</v>
@@ -2313,16 +2113,16 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
@@ -2333,16 +2133,16 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
         <v>1</v>
@@ -2353,7 +2153,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -2362,10 +2162,10 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16">
         <v>8</v>
@@ -2373,16 +2173,16 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
@@ -2393,16 +2193,16 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>1</v>
@@ -2413,7 +2213,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
@@ -2422,10 +2222,10 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <v>8</v>
@@ -2433,7 +2233,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -2442,10 +2242,10 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21">
         <v>8</v>

</xml_diff>